<commit_message>
add back in base web and fabric
</commit_message>
<xml_diff>
--- a/ExcelWebAddIn1/bin/Debug/Book1.xlsx
+++ b/ExcelWebAddIn1/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rcf9c2b51d31d4a6f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R31d5a62a965444b2"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="700" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R72edfbb51f8c458b"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R119c8ea408df4114"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b79d67f1-c306-48e2-84e9-db1ca55950a7}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9f2682e6-738c-4d4c-99e3-2213879165fc}">
   <we:reference id="ef16b601-2bed-45d3-8ecb-209e9042df76" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>